<commit_message>
calculos de los precios por lote, pero aun con errores
</commit_message>
<xml_diff>
--- a/data/raw/Bitacora.xlsx
+++ b/data/raw/Bitacora.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>fecha</t>
   </si>
@@ -22,28 +22,28 @@
     <t>lote</t>
   </si>
   <si>
-    <t>producto</t>
-  </si>
-  <si>
-    <t>variedad</t>
-  </si>
-  <si>
     <t>receta</t>
   </si>
   <si>
-    <t>cantidad</t>
+    <t>dimension_lote</t>
   </si>
   <si>
     <t>unidades</t>
   </si>
   <si>
-    <t>jabon</t>
+    <t>cantidad_productos</t>
   </si>
   <si>
-    <t>menta</t>
+    <t>1_balsamos</t>
+  </si>
+  <si>
+    <t>balsamo_alivia_2</t>
   </si>
   <si>
     <t>mL</t>
+  </si>
+  <si>
+    <t>jabon_menta_2</t>
   </si>
 </sst>
 </file>
@@ -51,10 +51,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -81,9 +81,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -96,13 +95,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -111,11 +103,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -127,42 +119,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -171,6 +127,35 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -186,24 +171,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -218,43 +218,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -266,139 +386,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -445,11 +445,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -486,6 +492,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -494,162 +509,147 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="8" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -985,18 +985,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75" outlineLevelRow="1" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75" outlineLevelRow="2" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="10.4"/>
+    <col min="3" max="3" width="13.3" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1015,31 +1016,44 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="2:6">
+      <c r="B2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="1">
-        <v>44160</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2">
+        <f>70*25</f>
+        <v>1750</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
       <c r="F2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1">
+        <v>44160</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3">
         <v>6890</v>
       </c>
-      <c r="G2" t="s">
-        <v>9</v>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3">
+        <f>13*3+16+8+12</f>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>